<commit_message>
Data simulacion matlab comparacion
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data MATLAB/Simulacion/DataSimMATLAB.xlsx
+++ b/comparisonFiles/Data MATLAB/Simulacion/DataSimMATLAB.xlsx
@@ -565,7 +565,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>0.19685945218759601</v>
       </c>
       <c r="I2" s="6">
-        <v>0.50392460823059004</v>
+        <v>0.80835738505953203</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>0.48336914653198998</v>
       </c>
       <c r="I3" s="6">
-        <v>0.50392484664916903</v>
+        <v>0.59145229122494702</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>0.38120481032020898</v>
       </c>
       <c r="I4" s="6">
-        <v>0.55666136741638095</v>
+        <v>0.52639073649588597</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>1.12375246728095</v>
       </c>
       <c r="I7" s="9">
-        <v>15.0640499591827</v>
+        <v>2.5210337555198099</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>0.809350567723366</v>
       </c>
       <c r="I10" s="9">
-        <v>2.2071149349212602</v>
+        <v>0.41737740556553699</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
         <v>0.96211852185043201</v>
       </c>
       <c r="I13" s="9">
-        <v>2.2149274349212602</v>
+        <v>0.54058373742891996</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -977,7 +977,7 @@
         <v>0.68702652329372305</v>
       </c>
       <c r="I14" s="9">
-        <v>1.8262414932250901</v>
+        <v>0.56066093329653799</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
         <v>1.3267946805478901</v>
       </c>
       <c r="I16" s="9">
-        <v>3.15637111663818</v>
+        <v>0.68684069528846103</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>0.83678875944907105</v>
       </c>
       <c r="I17" s="15">
-        <v>6.7981116771697998</v>
+        <v>0.675652400825275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglada data discreta matlab y scilab
</commit_message>
<xml_diff>
--- a/comparisonFiles/Data MATLAB/Simulacion/DataSimMATLAB.xlsx
+++ b/comparisonFiles/Data MATLAB/Simulacion/DataSimMATLAB.xlsx
@@ -559,7 +559,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H17"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
         <v>0.809350567723366</v>
       </c>
       <c r="I10" s="7">
-        <v>0.41737740556553699</v>
+        <v>0.48878500567329802</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>